<commit_message>
Update on 20250102 part 5
</commit_message>
<xml_diff>
--- a/各地组播源汇总/重庆.xlsx
+++ b/各地组播源汇总/重庆.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="79">
   <si>
     <t>联通组播</t>
   </si>
@@ -93,17 +93,9 @@
     <t>/udp/225.0.4.192:7980</t>
   </si>
   <si>
-    <t>重庆影视</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/udp/225.0.4.193:7980</t>
   </si>
   <si>
-    <t>重庆科教</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/udp/225.0.4.194:7980</t>
   </si>
   <si>
@@ -121,10 +113,6 @@
     <t>/udp/225.0.4.196:7980</t>
   </si>
   <si>
-    <t>重庆时尚生活</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/udp/225.0.4.189:7980</t>
   </si>
   <si>
@@ -166,9 +154,6 @@
     <t>电信组播</t>
   </si>
   <si>
-    <t>重庆影视</t>
-  </si>
-  <si>
     <t>/rtp/235.254.198.180:7980</t>
   </si>
   <si>
@@ -184,9 +169,6 @@
     <t>/rtp/235.254.196.199:7980</t>
   </si>
   <si>
-    <t>重庆科教</t>
-  </si>
-  <si>
     <t>/rtp/235.254.196.215:1132</t>
   </si>
   <si>
@@ -199,9 +181,6 @@
     <t>/rtp/235.254.196.210:1112</t>
   </si>
   <si>
-    <t>重庆时尚生活</t>
-  </si>
-  <si>
     <t>/rtp/235.254.198.182:7980</t>
   </si>
   <si>
@@ -300,6 +279,15 @@
   <si>
     <t>IP地址</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重庆影视剧</t>
+  </si>
+  <si>
+    <t>重庆红叶</t>
+  </si>
+  <si>
+    <t>重庆红岩文化</t>
   </si>
 </sst>
 </file>
@@ -881,7 +869,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
@@ -898,7 +886,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
@@ -915,7 +903,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
@@ -932,7 +920,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="B17" t="s">
         <v>2</v>
@@ -949,7 +937,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="B18" t="s">
         <v>2</v>
@@ -961,12 +949,12 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
         <v>2</v>
@@ -978,12 +966,12 @@
         <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="B20" t="s">
         <v>2</v>
@@ -995,12 +983,12 @@
         <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="B21" t="s">
         <v>2</v>
@@ -1012,12 +1000,12 @@
         <v>12</v>
       </c>
       <c r="E21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>2</v>
@@ -1029,12 +1017,12 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>2</v>
@@ -1046,12 +1034,12 @@
         <v>10</v>
       </c>
       <c r="E23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
         <v>2</v>
@@ -1063,12 +1051,12 @@
         <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
         <v>2</v>
@@ -1080,12 +1068,12 @@
         <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
         <v>2</v>
@@ -1097,12 +1085,12 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B27" t="s">
         <v>2</v>
@@ -1114,12 +1102,12 @@
         <v>10</v>
       </c>
       <c r="E27" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B28" t="s">
         <v>2</v>
@@ -1131,12 +1119,12 @@
         <v>11</v>
       </c>
       <c r="E28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B29" t="s">
         <v>2</v>
@@ -1148,12 +1136,12 @@
         <v>12</v>
       </c>
       <c r="E29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>78</v>
       </c>
       <c r="B30" t="s">
         <v>2</v>
@@ -1165,12 +1153,12 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>78</v>
       </c>
       <c r="B31" t="s">
         <v>2</v>
@@ -1182,12 +1170,12 @@
         <v>10</v>
       </c>
       <c r="E31" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>78</v>
       </c>
       <c r="B32" t="s">
         <v>2</v>
@@ -1199,12 +1187,12 @@
         <v>11</v>
       </c>
       <c r="E32" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>27</v>
+        <v>78</v>
       </c>
       <c r="B33" t="s">
         <v>2</v>
@@ -1216,12 +1204,12 @@
         <v>12</v>
       </c>
       <c r="E33" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B34" t="s">
         <v>2</v>
@@ -1233,12 +1221,12 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B35" t="s">
         <v>2</v>
@@ -1250,12 +1238,12 @@
         <v>10</v>
       </c>
       <c r="E35" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B36" t="s">
         <v>2</v>
@@ -1267,12 +1255,12 @@
         <v>11</v>
       </c>
       <c r="E36" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B37" t="s">
         <v>2</v>
@@ -1284,12 +1272,12 @@
         <v>12</v>
       </c>
       <c r="E37" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B38" t="s">
         <v>2</v>
@@ -1301,12 +1289,12 @@
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B39" t="s">
         <v>2</v>
@@ -1318,12 +1306,12 @@
         <v>10</v>
       </c>
       <c r="E39" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B40" t="s">
         <v>2</v>
@@ -1335,12 +1323,12 @@
         <v>11</v>
       </c>
       <c r="E40" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B41" t="s">
         <v>2</v>
@@ -1352,12 +1340,12 @@
         <v>12</v>
       </c>
       <c r="E41" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B42" t="s">
         <v>2</v>
@@ -1369,12 +1357,12 @@
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B43" t="s">
         <v>2</v>
@@ -1386,12 +1374,12 @@
         <v>10</v>
       </c>
       <c r="E43" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B44" t="s">
         <v>2</v>
@@ -1403,12 +1391,12 @@
         <v>11</v>
       </c>
       <c r="E44" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B45" t="s">
         <v>2</v>
@@ -1420,7 +1408,7 @@
         <v>12</v>
       </c>
       <c r="E45" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1450,937 +1438,937 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D6" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D9" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D10" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D12" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D13" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E13" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D14" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D15" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C16" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E16" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D17" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E17" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D18" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E18" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E19" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D20" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E20" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C21" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D21" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E21" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C22" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E22" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C23" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D23" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E23" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C24" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D24" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E24" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="B25" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D25" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E25" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C26" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D26" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E26" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C27" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D27" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E27" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="B28" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C28" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D28" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E28" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B29" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C29" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D29" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E29" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B30" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C30" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D30" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E30" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B31" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C31" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D31" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E31" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B32" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D32" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E32" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B33" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C33" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D33" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E33" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B34" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C34" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D34" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E34" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B35" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C35" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D35" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E35" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B36" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C36" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D36" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E36" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C37" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D37" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E37" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B38" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C38" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D38" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E38" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B39" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C39" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D39" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E39" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B40" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C40" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D40" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E40" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B41" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C41" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D41" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E41" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B42" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C42" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D42" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E42" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B43" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C43" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D43" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E43" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B44" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C44" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D44" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E44" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B45" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C45" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D45" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E45" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B46" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C46" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D46" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E46" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47" t="s">
+        <v>66</v>
+      </c>
+      <c r="C47" t="s">
+        <v>71</v>
+      </c>
+      <c r="D47" t="s">
         <v>64</v>
       </c>
-      <c r="B47" t="s">
-        <v>72</v>
-      </c>
-      <c r="C47" t="s">
-        <v>77</v>
-      </c>
-      <c r="D47" t="s">
-        <v>70</v>
-      </c>
       <c r="E47" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B48" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C48" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D48" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E48" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B49" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C49" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D49" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E49" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B50" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C50" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D50" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E50" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B51" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C51" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D51" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E51" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B52" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C52" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D52" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E52" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B53" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C53" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D53" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E53" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B54" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C54" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D54" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E54" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B55" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C55" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D55" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E55" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2409,36 +2397,36 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>